<commit_message>
Se importo nuevos archivos
</commit_message>
<xml_diff>
--- a/archivos de importación/alumno.xlsx
+++ b/archivos de importación/alumno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6cbe82d14fb70d01/Documentos/CESMI/Tercer AÑO/Seminario de Análisis/Gestion_de_Asistencia_Escolar/archivos de importación/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_085D0F6F9270C00E623554765827DEB9ABB59DF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B30F564-FE2B-4376-B052-FFEE28D06907}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_085D0F6F9270C00E623554765827DEB9ABB59DF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{307388AC-18E9-42A2-A175-B19B5D0F802C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>nombre</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="E5:J13"/>
+      <selection activeCell="A2" sqref="A2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,11 +501,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -519,9 +516,6 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -546,11 +540,8 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -564,9 +555,6 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -580,7 +568,7 @@
       <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -588,11 +576,8 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
@@ -606,9 +591,6 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -633,11 +615,8 @@
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -647,7 +626,7 @@
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>27</v>
       </c>
       <c r="F12" t="s">
@@ -667,7 +646,7 @@
       <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ME FALTA POCO PARA TERMINAR
</commit_message>
<xml_diff>
--- a/archivos de importación/alumno.xlsx
+++ b/archivos de importación/alumno.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6cbe82d14fb70d01/Documentos/CESMI/Tercer AÑO/Seminario de Análisis/Gestion_de_Asistencia_Escolar/archivos de importación/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_085D0F6F9270C00E623554765827DEB9ABB59DF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CEE8836-B0C0-4F38-ABD1-5C27FA223E8C}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_085D0F6F9270C00E623554765827DEB9ABB59DF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BADD787-7031-4A2E-BF5B-B19CF74168EB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="alumno" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,12 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>fecha de nacimiento</t>
-  </si>
-  <si>
     <t>Carrera</t>
   </si>
   <si>
@@ -110,13 +104,19 @@
   </si>
   <si>
     <t xml:space="preserve">Administración de empresas </t>
+  </si>
+  <si>
+    <t>Fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>Nombre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +135,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,49 +194,38 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,304 +531,231 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="4"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="4"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="C4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="C5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
+      <c r="C8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="C10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
+      <c r="B11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="C12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="B13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="5">
+        <v>24</v>
+      </c>
+      <c r="B14" s="8">
         <v>37061</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="C14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="5">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8">
         <v>37427</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="C15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C2:E2"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>